<commit_message>
SZ, LU, OW, VD
</commit_message>
<xml_diff>
--- a/SZ_nais_einheiten_unique_bh_20241128_mf_bh.xlsx
+++ b/SZ_nais_einheiten_unique_bh_20241128_mf_bh.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CCW24sensi\SZ_Herbst_anfragen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\develops\sensitivewaldstandorteCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59B658D0-8146-49A9-9701-F18C06734E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B4DFBF-4DA1-4634-99A5-2603185018C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
     <sheet name="Read me" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$M$86</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="162">
   <si>
     <t>SZ Einheit</t>
   </si>
@@ -360,12 +363,6 @@
     <t>Bemerkungen bh</t>
   </si>
   <si>
-    <t>tahs inkl. co</t>
-  </si>
-  <si>
-    <t>tahs ohne co</t>
-  </si>
-  <si>
     <t>hm sa osa</t>
   </si>
   <si>
@@ -405,15 +402,6 @@
     <t>53(48)</t>
   </si>
   <si>
-    <t>Bedingung Höhenstufe</t>
-  </si>
-  <si>
-    <t>NaiS</t>
-  </si>
-  <si>
-    <t>Höhenstufe (ohne collin)</t>
-  </si>
-  <si>
     <t>Bemerkung Monika</t>
   </si>
   <si>
@@ -508,6 +496,33 @@
   </si>
   <si>
     <t>solche Ausreisser erzeugen dann wahrscheinlich leere Flächen, ich kann es dann versuchen zu korrigieren (SZ ist eigenltich abgeschlossen, sie wollen aber eine Vereinfachung mit den Standorttypengruppen und die Entwässerungen müssen wir noch einbauen</t>
+  </si>
+  <si>
+    <t>nais</t>
+  </si>
+  <si>
+    <t>hs_ohne_co</t>
+  </si>
+  <si>
+    <t>hs_inkl_co</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>nais1</t>
+  </si>
+  <si>
+    <t>nais2</t>
+  </si>
+  <si>
+    <t>57Bl</t>
+  </si>
+  <si>
+    <t>60*TA</t>
+  </si>
+  <si>
+    <t>Bedingung_Hoehenstufe</t>
   </si>
 </sst>
 </file>
@@ -599,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -612,10 +627,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -918,23 +934,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F71FBD-9755-47D8-92CE-BD3A03C07C52}">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" customWidth="1"/>
-    <col min="4" max="5" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="117.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="235" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -945,31 +968,37 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>13</v>
       </c>
@@ -985,14 +1014,19 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I2" s="8" t="str">
+        <f>H2</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>16</v>
       </c>
@@ -1008,14 +1042,19 @@
       <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="8" t="str">
+        <f t="shared" ref="I3:I66" si="0">H3</f>
+        <v>6</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -1031,14 +1070,19 @@
       <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>7a</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -1054,14 +1098,19 @@
       <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>8a</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>25</v>
       </c>
@@ -1077,14 +1126,19 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>9a</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>34</v>
       </c>
@@ -1100,14 +1154,19 @@
       <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>10a</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>39</v>
       </c>
@@ -1123,14 +1182,19 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43</v>
       </c>
@@ -1146,14 +1210,19 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>12a</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>49</v>
       </c>
@@ -1172,14 +1241,19 @@
       <c r="G10" t="s">
         <v>3</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>13a</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>49</v>
       </c>
@@ -1189,14 +1263,19 @@
       <c r="G11" t="s">
         <v>45</v>
       </c>
-      <c r="H11" t="s">
-        <v>147</v>
-      </c>
-      <c r="I11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>13h</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>30</v>
       </c>
@@ -1212,14 +1291,19 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>63</v>
       </c>
@@ -1235,14 +1319,19 @@
       <c r="E13" t="s">
         <v>3</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>53</v>
       </c>
@@ -1258,14 +1347,19 @@
       <c r="E14" t="s">
         <v>24</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>60</v>
       </c>
@@ -1281,14 +1375,19 @@
       <c r="E15" t="s">
         <v>17</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>73</v>
       </c>
@@ -1304,14 +1403,19 @@
       <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>98</v>
       </c>
@@ -1327,14 +1431,19 @@
       <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>74</v>
       </c>
@@ -1350,14 +1459,19 @@
       <c r="E18" t="s">
         <v>45</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I18" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>66</v>
       </c>
@@ -1373,14 +1487,19 @@
       <c r="E19" t="s">
         <v>81</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>144</v>
       </c>
@@ -1396,14 +1515,19 @@
       <c r="E20" t="s">
         <v>37</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="K20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>69</v>
       </c>
@@ -1419,14 +1543,19 @@
       <c r="E21" t="s">
         <v>7</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>130</v>
       </c>
@@ -1442,14 +1571,19 @@
       <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I22" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J22" s="8"/>
+      <c r="K22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>149</v>
       </c>
@@ -1465,14 +1599,19 @@
       <c r="E23" t="s">
         <v>17</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I23" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="J23" s="8"/>
+      <c r="K23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>161</v>
       </c>
@@ -1480,7 +1619,7 @@
         <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
@@ -1488,20 +1627,25 @@
       <c r="E24" t="s">
         <v>3</v>
       </c>
-      <c r="H24" t="s">
-        <v>136</v>
-      </c>
-      <c r="I24" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" t="s">
-        <v>137</v>
-      </c>
+      <c r="H24" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I24" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>27f</v>
+      </c>
+      <c r="J24" s="8"/>
       <c r="K24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="L24" t="s">
+        <v>132</v>
+      </c>
+      <c r="M24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -1517,20 +1661,25 @@
       <c r="E25" t="s">
         <v>3</v>
       </c>
-      <c r="H25" t="s">
-        <v>128</v>
-      </c>
-      <c r="I25" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" t="s">
-        <v>129</v>
-      </c>
+      <c r="H25" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>29A</v>
+      </c>
+      <c r="J25" s="8"/>
       <c r="K25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="L25" t="s">
+        <v>124</v>
+      </c>
+      <c r="M25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>7</v>
       </c>
@@ -1546,14 +1695,19 @@
       <c r="E26" t="s">
         <v>17</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="8">
         <v>30</v>
       </c>
-      <c r="I26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I26" s="8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>95</v>
       </c>
@@ -1569,14 +1723,19 @@
       <c r="E27" t="s">
         <v>42</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="J27" s="8"/>
+      <c r="K27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>192</v>
       </c>
@@ -1587,25 +1746,30 @@
         <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E28" t="s">
-        <v>120</v>
-      </c>
-      <c r="H28" t="s">
+        <v>118</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="J28" s="8"/>
+      <c r="K28" t="s">
         <v>42</v>
       </c>
-      <c r="J28" t="s">
-        <v>138</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>96</v>
       </c>
@@ -1621,44 +1785,61 @@
       <c r="E29" t="s">
         <v>42</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="J29" s="8"/>
+      <c r="K29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>151</v>
-      </c>
-      <c r="H30" t="s">
-        <v>151</v>
-      </c>
-      <c r="I30" t="s">
-        <v>45</v>
-      </c>
-      <c r="J30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K30" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>152</v>
-      </c>
-      <c r="H31" t="s">
-        <v>152</v>
-      </c>
-      <c r="I31" t="s">
+        <v>147</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K31" t="s">
         <v>81</v>
       </c>
-      <c r="J31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>204</v>
       </c>
@@ -1674,14 +1855,19 @@
       <c r="E32" t="s">
         <v>81</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J32" s="8"/>
+      <c r="K32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>212</v>
       </c>
@@ -1697,14 +1883,19 @@
       <c r="E33" t="s">
         <v>81</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="J33" s="8"/>
+      <c r="K33" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>215</v>
       </c>
@@ -1712,7 +1903,7 @@
         <v>84</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>42</v>
@@ -1723,14 +1914,19 @@
       <c r="G34" t="s">
         <v>42</v>
       </c>
-      <c r="H34" t="s">
-        <v>121</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="H34" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>53Ta</v>
+      </c>
+      <c r="J34" s="8"/>
+      <c r="K34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>215</v>
       </c>
@@ -1744,19 +1940,24 @@
         <v>10</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G35" t="s">
         <v>10</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="J35" s="8"/>
+      <c r="K35" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>230</v>
       </c>
@@ -1772,14 +1973,19 @@
       <c r="E36" t="s">
         <v>42</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="J36" s="8"/>
+      <c r="K36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>239</v>
       </c>
@@ -1795,14 +2001,19 @@
       <c r="E37" t="s">
         <v>10</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="J37" s="8"/>
+      <c r="K37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>254</v>
       </c>
@@ -1818,14 +2029,19 @@
       <c r="E38" t="s">
         <v>3</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="J38" s="8"/>
+      <c r="K38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>257</v>
       </c>
@@ -1841,14 +2057,19 @@
       <c r="E39" t="s">
         <v>37</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="J39" s="8"/>
+      <c r="K39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>4</v>
       </c>
@@ -1864,20 +2085,25 @@
       <c r="E40" t="s">
         <v>7</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I40" t="s">
-        <v>133</v>
-      </c>
-      <c r="J40" t="s">
-        <v>134</v>
-      </c>
+      <c r="I40" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="J40" s="8"/>
       <c r="K40" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="L40" t="s">
+        <v>129</v>
+      </c>
+      <c r="M40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>5</v>
       </c>
@@ -1893,14 +2119,19 @@
       <c r="E41" t="s">
         <v>5</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I41" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I41" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="J41" s="8"/>
+      <c r="K41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -1916,14 +2147,19 @@
       <c r="E42" t="s">
         <v>7</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I42" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I42" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="J42" s="8"/>
+      <c r="K42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -1934,25 +2170,30 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H43" t="s">
+        <v>108</v>
+      </c>
+      <c r="H43" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J43" t="s">
-        <v>130</v>
-      </c>
+      <c r="I43" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="J43" s="8"/>
       <c r="K43" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+      <c r="L43" t="s">
+        <v>125</v>
+      </c>
+      <c r="M43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>6</v>
       </c>
@@ -1968,20 +2209,25 @@
       <c r="E44" t="s">
         <v>10</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="8">
         <v>69</v>
       </c>
-      <c r="I44" t="s">
-        <v>133</v>
-      </c>
-      <c r="J44" t="s">
-        <v>127</v>
-      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="J44" s="8"/>
       <c r="K44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="L44" t="s">
+        <v>122</v>
+      </c>
+      <c r="M44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>27</v>
       </c>
@@ -1997,14 +2243,19 @@
       <c r="E45" t="s">
         <v>17</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I45" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>13e</v>
+      </c>
+      <c r="J45" s="8"/>
+      <c r="K45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>85</v>
       </c>
@@ -2020,14 +2271,19 @@
       <c r="E46" t="s">
         <v>45</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I46" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>18*</v>
+      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>78</v>
       </c>
@@ -2043,14 +2299,20 @@
       <c r="E47" t="s">
         <v>45</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I47" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>70</v>
       </c>
@@ -2066,14 +2328,19 @@
       <c r="E48" t="s">
         <v>45</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I48" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I48" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>18M</v>
+      </c>
+      <c r="J48" s="8"/>
+      <c r="K48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>91</v>
       </c>
@@ -2089,17 +2356,22 @@
       <c r="E49" t="s">
         <v>45</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I49" t="s">
-        <v>45</v>
-      </c>
-      <c r="J49" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I49" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>18v</v>
+      </c>
+      <c r="J49" s="8"/>
+      <c r="K49" t="s">
+        <v>45</v>
+      </c>
+      <c r="L49" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>72</v>
       </c>
@@ -2115,17 +2387,22 @@
       <c r="E50" t="s">
         <v>45</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I50" t="s">
-        <v>45</v>
-      </c>
-      <c r="J50" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I50" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>18w</v>
+      </c>
+      <c r="J50" s="8"/>
+      <c r="K50" t="s">
+        <v>45</v>
+      </c>
+      <c r="L50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>110</v>
       </c>
@@ -2141,14 +2418,19 @@
       <c r="E51" t="s">
         <v>45</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I51" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I51" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>19f</v>
+      </c>
+      <c r="J51" s="8"/>
+      <c r="K51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>107</v>
       </c>
@@ -2164,14 +2446,19 @@
       <c r="E52" t="s">
         <v>45</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I52" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I52" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>20E</v>
+      </c>
+      <c r="J52" s="8"/>
+      <c r="K52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>128</v>
       </c>
@@ -2187,14 +2474,19 @@
       <c r="E53" t="s">
         <v>7</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>24*</v>
+      </c>
+      <c r="J53" s="8"/>
+      <c r="K53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>135</v>
       </c>
@@ -2210,14 +2502,19 @@
       <c r="E54" t="s">
         <v>17</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I54" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>25F</v>
+      </c>
+      <c r="J54" s="8"/>
+      <c r="K54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>137</v>
       </c>
@@ -2233,14 +2530,19 @@
       <c r="E55" t="s">
         <v>17</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I55" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I55" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>25F</v>
+      </c>
+      <c r="J55" s="8"/>
+      <c r="K55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>154</v>
       </c>
@@ -2256,14 +2558,19 @@
       <c r="E56" t="s">
         <v>42</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>26h</v>
+      </c>
+      <c r="J56" s="8"/>
+      <c r="K56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>156</v>
       </c>
@@ -2279,14 +2586,19 @@
       <c r="E57" t="s">
         <v>45</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I57" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I57" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>26w</v>
+      </c>
+      <c r="J57" s="8"/>
+      <c r="K57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>112</v>
       </c>
@@ -2305,14 +2617,19 @@
       <c r="G58" t="s">
         <v>45</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="I58" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I58" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>27h</v>
+      </c>
+      <c r="J58" s="8"/>
+      <c r="K58" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>112</v>
       </c>
@@ -2322,14 +2639,19 @@
       <c r="G59" t="s">
         <v>81</v>
       </c>
-      <c r="H59" t="s">
-        <v>148</v>
-      </c>
-      <c r="I59" t="s">
+      <c r="H59" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I59" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>27*</v>
+      </c>
+      <c r="J59" s="8"/>
+      <c r="K59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>171</v>
       </c>
@@ -2340,22 +2662,28 @@
         <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G60" t="s">
         <v>45</v>
       </c>
-      <c r="H60" t="s">
-        <v>150</v>
-      </c>
-      <c r="I60" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H60" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>171</v>
       </c>
@@ -2365,14 +2693,20 @@
       <c r="G61" t="s">
         <v>81</v>
       </c>
-      <c r="H61" t="s">
-        <v>149</v>
-      </c>
-      <c r="I61" t="s">
+      <c r="H61" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K61" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>12</v>
       </c>
@@ -2380,7 +2714,7 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D62" t="s">
         <v>3</v>
@@ -2389,19 +2723,24 @@
         <v>17</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G62" t="s">
         <v>3</v>
       </c>
-      <c r="H62" t="s">
-        <v>111</v>
-      </c>
-      <c r="I62" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H62" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I62" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>32C</v>
+      </c>
+      <c r="J62" s="8"/>
+      <c r="K62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>12</v>
       </c>
@@ -2418,19 +2757,24 @@
         <v>7</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G63" t="s">
         <v>7</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>32V</v>
+      </c>
+      <c r="J63" s="8"/>
+      <c r="K63" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>10</v>
       </c>
@@ -2446,14 +2790,19 @@
       <c r="E64" t="s">
         <v>17</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I64" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>40*</v>
+      </c>
+      <c r="J64" s="8"/>
+      <c r="K64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>94</v>
       </c>
@@ -2469,14 +2818,19 @@
       <c r="E65" t="s">
         <v>42</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I65" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>46*</v>
+      </c>
+      <c r="J65" s="8"/>
+      <c r="K65" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>187</v>
       </c>
@@ -2492,14 +2846,19 @@
       <c r="E66" t="s">
         <v>81</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I66" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>46M</v>
+      </c>
+      <c r="J66" s="8"/>
+      <c r="K66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>190</v>
       </c>
@@ -2515,20 +2874,26 @@
       <c r="E67" t="s">
         <v>42</v>
       </c>
-      <c r="H67" t="s">
-        <v>141</v>
-      </c>
-      <c r="I67" t="s">
+      <c r="H67" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K67" t="s">
         <v>42</v>
       </c>
-      <c r="J67" t="s">
-        <v>142</v>
-      </c>
-      <c r="K67" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L67" t="s">
+        <v>137</v>
+      </c>
+      <c r="M67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>195</v>
       </c>
@@ -2544,20 +2909,25 @@
       <c r="E68" t="s">
         <v>42</v>
       </c>
-      <c r="H68" t="s">
-        <v>143</v>
-      </c>
-      <c r="I68" t="s">
+      <c r="H68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="I68" s="8" t="str">
+        <f t="shared" ref="I67:I86" si="1">H68</f>
+        <v>49*Ta</v>
+      </c>
+      <c r="J68" s="8"/>
+      <c r="K68" t="s">
         <v>81</v>
       </c>
-      <c r="J68" t="s">
-        <v>144</v>
-      </c>
-      <c r="K68" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L68" t="s">
+        <v>139</v>
+      </c>
+      <c r="M68" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>209</v>
       </c>
@@ -2573,14 +2943,19 @@
       <c r="E69" t="s">
         <v>81</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>50*</v>
+      </c>
+      <c r="J69" s="8"/>
+      <c r="K69" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>223</v>
       </c>
@@ -2599,14 +2974,20 @@
       <c r="G70" t="s">
         <v>42</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K70" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>223</v>
       </c>
@@ -2614,31 +2995,37 @@
         <v>85</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G71" t="s">
         <v>10</v>
       </c>
-      <c r="H71" t="s">
-        <v>145</v>
-      </c>
-      <c r="I71" t="s">
+      <c r="H71" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="K71" t="s">
         <v>10</v>
       </c>
-      <c r="J71" t="s">
-        <v>146</v>
-      </c>
-      <c r="K71" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L71" t="s">
+        <v>141</v>
+      </c>
+      <c r="M71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>174</v>
       </c>
@@ -2652,19 +3039,25 @@
         <v>10</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G72" t="s">
         <v>10</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J72" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K72" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>174</v>
       </c>
@@ -2672,7 +3065,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>81</v>
@@ -2683,14 +3076,20 @@
       <c r="G73" t="s">
         <v>81</v>
       </c>
-      <c r="H73" t="s">
-        <v>118</v>
-      </c>
-      <c r="I73" t="s">
+      <c r="H73" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I73" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J73" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K73" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>238</v>
       </c>
@@ -2706,14 +3105,19 @@
       <c r="E74" t="s">
         <v>10</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H74" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>57C</v>
+      </c>
+      <c r="J74" s="8"/>
+      <c r="K74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>231</v>
       </c>
@@ -2729,14 +3133,19 @@
       <c r="E75" t="s">
         <v>10</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H75" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>57S</v>
+      </c>
+      <c r="J75" s="8"/>
+      <c r="K75" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>236</v>
       </c>
@@ -2752,14 +3161,19 @@
       <c r="E76" t="s">
         <v>10</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>57V</v>
+      </c>
+      <c r="J76" s="8"/>
+      <c r="K76" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>175</v>
       </c>
@@ -2773,19 +3187,24 @@
         <v>10</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G77" t="s">
         <v>10</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H77" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>60*</v>
+      </c>
+      <c r="J77" s="8"/>
+      <c r="K77" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>175</v>
       </c>
@@ -2793,7 +3212,7 @@
         <v>74</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>42</v>
@@ -2804,14 +3223,19 @@
       <c r="G78" t="s">
         <v>42</v>
       </c>
-      <c r="H78" t="s">
-        <v>119</v>
-      </c>
-      <c r="I78" t="s">
+      <c r="H78" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I78" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>60*Ta</v>
+      </c>
+      <c r="J78" s="8"/>
+      <c r="K78" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>249</v>
       </c>
@@ -2827,14 +3251,19 @@
       <c r="E79" t="s">
         <v>10</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H79" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I79" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>60A</v>
+      </c>
+      <c r="J79" s="8"/>
+      <c r="K79" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>250</v>
       </c>
@@ -2850,14 +3279,19 @@
       <c r="E80" t="s">
         <v>10</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>60E</v>
+      </c>
+      <c r="J80" s="8"/>
+      <c r="K80" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>261</v>
       </c>
@@ -2873,14 +3307,20 @@
       <c r="E81" t="s">
         <v>37</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J81" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K81" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>256</v>
       </c>
@@ -2896,14 +3336,20 @@
       <c r="E82" t="s">
         <v>17</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H82" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="I82" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I82" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J82" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K82" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>262</v>
       </c>
@@ -2919,14 +3365,19 @@
       <c r="E83" t="s">
         <v>7</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I83" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>67G</v>
+      </c>
+      <c r="J83" s="8"/>
+      <c r="K83" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>264</v>
       </c>
@@ -2942,14 +3393,19 @@
       <c r="E84" t="s">
         <v>5</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I84" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>69G</v>
+      </c>
+      <c r="J84" s="8"/>
+      <c r="K84" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>265</v>
       </c>
@@ -2965,14 +3421,19 @@
       <c r="E85" t="s">
         <v>7</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H85" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>71G</v>
+      </c>
+      <c r="J85" s="8"/>
+      <c r="K85" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>268</v>
       </c>
@@ -2988,15 +3449,21 @@
       <c r="E86" t="s">
         <v>7</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H86" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>AV</v>
+      </c>
+      <c r="J86" s="8"/>
+      <c r="K86" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J86">
+  <autoFilter ref="A1:M86" xr:uid="{69F71FBD-9755-47D8-92CE-BD3A03C07C52}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L86">
     <sortCondition ref="B2:B86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3011,11 +3478,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>